<commit_message>
tareas y standup metting
</commit_message>
<xml_diff>
--- a/Semana 31 agosto - 4 septiembre/Stand_Up_Meeitng_Week_2.xlsx
+++ b/Semana 31 agosto - 4 septiembre/Stand_Up_Meeitng_Week_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mythe\Documents\GitHub\Ingenieria_Software\Semana 31 agosto - 4 septiembre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B187ACA-6493-4328-B45A-BCB01874C653}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A294E7-249B-482C-9C1D-30CB74E8DB21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3320EE79-9243-42E8-8E5F-EF80DE6A9110}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
   <si>
     <t xml:space="preserve"> MIEMBRO</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Exploner lo planteado y tomar las sugerencias del profe</t>
+  </si>
+  <si>
+    <t>Reunion semanal y asignacion de tareas</t>
   </si>
 </sst>
 </file>
@@ -744,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4E8726-24EF-4B21-B937-D55FA5E6EA95}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,7 +759,7 @@
     <col min="4" max="4" width="85.42578125" customWidth="1"/>
     <col min="5" max="5" width="94.42578125" customWidth="1"/>
     <col min="6" max="6" width="54" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="38.7109375" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" customWidth="1"/>
@@ -877,7 +880,9 @@
       <c r="F7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
@@ -896,7 +901,9 @@
       <c r="F8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
@@ -915,7 +922,9 @@
       <c r="F9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">

</xml_diff>